<commit_message>
Talent damage accurate improved
- Add monster res and level setting
- Add tooltip to show tip about each damage
- Fix attack_talents.xlsx file that make program error (forgot to change '/' to '&')
- Toplevel now can move by left click
- Change 'geometry('0x0')' to 'withdraw' to make it easy to hide and show
</commit_message>
<xml_diff>
--- a/data/characters_weapons.xlsx
+++ b/data/characters_weapons.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nonext\PycharmProjects\GenshinAutoInfo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F83E88C-3D66-4644-B185-8B64186121E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A462B3D-B512-4173-9E4E-59A35801F49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="945" windowWidth="27060" windowHeight="12900" xr2:uid="{3810FFE1-224D-423A-BB9B-1B42AE957ECD}"/>
+    <workbookView xWindow="11265" yWindow="930" windowWidth="20715" windowHeight="12645" activeTab="1" xr2:uid="{3810FFE1-224D-423A-BB9B-1B42AE957ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4240" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4240" uniqueCount="746">
   <si>
     <t>Name</t>
   </si>
@@ -2252,6 +2252,21 @@
   <si>
     <t>Anemo</t>
   </si>
+  <si>
+    <t>Traveler Female Anemo1</t>
+  </si>
+  <si>
+    <t>Traveler Male Geo1</t>
+  </si>
+  <si>
+    <t>Traveler Female Geo1</t>
+  </si>
+  <si>
+    <t>Traveler Male Electro1</t>
+  </si>
+  <si>
+    <t>Traveler Female Electro1</t>
+  </si>
 </sst>
 </file>
 
@@ -2657,10 +2672,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{038FAB3E-861B-4298-8601-A64071A2442D}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y735"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A696" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y720" sqref="Y720"/>
+    <sheetView topLeftCell="A672" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D676" sqref="D676"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31889,7 +31905,7 @@
     </row>
     <row r="658" spans="1:25">
       <c r="A658" s="1" t="s">
-        <v>302</v>
+        <v>741</v>
       </c>
       <c r="B658" s="2"/>
       <c r="C658" s="2">
@@ -32572,7 +32588,7 @@
     </row>
     <row r="674" spans="1:25">
       <c r="A674" s="1" t="s">
-        <v>302</v>
+        <v>742</v>
       </c>
       <c r="B674" s="2"/>
       <c r="C674" s="2">
@@ -33255,7 +33271,7 @@
     </row>
     <row r="690" spans="1:25">
       <c r="A690" s="1" t="s">
-        <v>302</v>
+        <v>743</v>
       </c>
       <c r="B690" s="2"/>
       <c r="C690" s="2">
@@ -33938,7 +33954,7 @@
     </row>
     <row r="706" spans="1:25">
       <c r="A706" s="1" t="s">
-        <v>302</v>
+        <v>744</v>
       </c>
       <c r="B706" s="2"/>
       <c r="C706" s="2">
@@ -34621,7 +34637,7 @@
     </row>
     <row r="722" spans="1:25">
       <c r="A722" s="1" t="s">
-        <v>302</v>
+        <v>745</v>
       </c>
       <c r="B722" s="2"/>
       <c r="C722" s="2">
@@ -35235,10 +35251,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08AF9DC4-53FD-4361-AD1D-012FA0AF03B8}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M3239"/>
   <sheetViews>
-    <sheetView topLeftCell="A2015" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1379" sqref="A1379"/>
+    <sheetView tabSelected="1" topLeftCell="A460" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E485" sqref="E485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -72995,6 +73012,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733B8F90-BDB2-47F8-BA3C-192D9B49345E}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -73685,6 +73703,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2C99BA-3ABA-4330-B226-6C2C9730B3D6}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">

</xml_diff>

<commit_message>
Ex.Tartaglia all dmg works without problem
- remove 'set_color' from each file and make it global function that can call by 'function.set_witget_color'
- finish weapon stats update
- change lv position of Character's class to match with excel file
</commit_message>
<xml_diff>
--- a/data/characters_weapons.xlsx
+++ b/data/characters_weapons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nonext\PycharmProjects\GenshinAutoInfo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A462B3D-B512-4173-9E4E-59A35801F49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246031D0-84F0-4542-89F0-7A8A8A27317A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11265" yWindow="930" windowWidth="20715" windowHeight="12645" activeTab="1" xr2:uid="{3810FFE1-224D-423A-BB9B-1B42AE957ECD}"/>
+    <workbookView xWindow="12885" yWindow="1995" windowWidth="24390" windowHeight="13515" xr2:uid="{3810FFE1-224D-423A-BB9B-1B42AE957ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="5" r:id="rId1"/>
@@ -2675,8 +2675,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y735"/>
   <sheetViews>
-    <sheetView topLeftCell="A672" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D676" sqref="D676"/>
+    <sheetView tabSelected="1" topLeftCell="A401" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X402" sqref="X402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -35254,7 +35254,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M3239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A460" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A460" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E485" sqref="E485"/>
     </sheetView>
   </sheetViews>

</xml_diff>